<commit_message>
Changes of 27th july 2022
</commit_message>
<xml_diff>
--- a/Connect/src/main/resources/connect_TestData/sample_order_creation.xlsx
+++ b/Connect/src/main/resources/connect_TestData/sample_order_creation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="138">
   <si>
     <t>Caller</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>3431254</t>
+  </si>
+  <si>
+    <t>766</t>
   </si>
 </sst>
 </file>
@@ -984,20 +987,20 @@
       <c r="Y2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>49</v>
+      <c r="Z2" t="s">
+        <v>129</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>50</v>
+      <c r="AB2" t="s">
+        <v>53</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>51</v>
+      <c r="AD2" t="s">
+        <v>137</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>52</v>

</xml_diff>